<commit_message>
Use of fill between for positive and negative difference only
</commit_message>
<xml_diff>
--- a/Results_4_FigS5-11.xlsx
+++ b/Results_4_FigS5-11.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pierrebedoucha/SourceTree/ml_tunnels/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1685DFDC-A1E5-5F4A-8B5C-5B7203ED11FE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40634F48-A159-3D40-82EB-28B263CCE27E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-60" yWindow="460" windowWidth="28860" windowHeight="17020" xr2:uid="{ED3F7AC0-6C4A-2845-B94D-9D2C4A69414D}"/>
   </bookViews>
@@ -310,7 +310,7 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{79450D51-A913-F144-AD62-06238DC4CE36}" name="Table1" displayName="Table1" ref="A10:AI17" totalsRowShown="0">
   <autoFilter ref="A10:AI17" xr:uid="{78E1E120-4779-D145-9E01-8890B903D226}">
-    <filterColumn colId="15">
+    <filterColumn colId="14">
       <filters>
         <filter val="1"/>
       </filters>
@@ -360,7 +360,7 @@
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3DF26DCD-855B-3E4D-AE0C-C5BD95EE8342}" name="Table2" displayName="Table2" ref="A1:AI8" totalsRowShown="0">
   <autoFilter ref="A1:AI8" xr:uid="{E0B025A3-8438-E54C-9F98-74A2817F9EAE}">
-    <filterColumn colId="15">
+    <filterColumn colId="14">
       <filters>
         <filter val="1"/>
       </filters>
@@ -410,7 +410,7 @@
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{AD6D32EC-78D0-CD49-8DB5-DDEA7D322B89}" name="Table3" displayName="Table3" ref="A19:AI25" totalsRowShown="0">
   <autoFilter ref="A19:AI25" xr:uid="{5DEAEDB8-41C5-D147-80F4-E48ECA27DB41}">
-    <filterColumn colId="15">
+    <filterColumn colId="14">
       <filters>
         <filter val="1"/>
       </filters>
@@ -460,7 +460,7 @@
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{8035B28C-2409-E449-81FA-D399D358795A}" name="Table4" displayName="Table4" ref="A27:AI34" totalsRowShown="0">
   <autoFilter ref="A27:AI34" xr:uid="{CB89E674-5EE8-AA48-BE26-E5495B1AE672}">
-    <filterColumn colId="15">
+    <filterColumn colId="14">
       <filters>
         <filter val="1"/>
       </filters>
@@ -510,12 +510,7 @@
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{27EC72F9-CA3E-B442-B108-24742682A2E4}" name="Table5" displayName="Table5" ref="A36:AI43" totalsRowShown="0">
   <autoFilter ref="A36:AI43" xr:uid="{CD505A0B-D089-AC41-AC48-5695AE99FF43}">
-    <filterColumn colId="8">
-      <filters>
-        <filter val="1"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="15">
+    <filterColumn colId="14">
       <filters>
         <filter val="1"/>
       </filters>
@@ -565,12 +560,7 @@
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{FE37AA6E-F8F1-CC48-ADA5-B32BD3D61C85}" name="Table6" displayName="Table6" ref="A45:AI52" totalsRowShown="0">
   <autoFilter ref="A45:AI52" xr:uid="{C69B9523-DEC1-1D40-A68C-FA8B2400D7C6}">
-    <filterColumn colId="11">
-      <filters>
-        <filter val="1"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="15">
+    <filterColumn colId="14">
       <filters>
         <filter val="1"/>
       </filters>
@@ -917,7 +907,7 @@
   <dimension ref="A1:AI52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1"/>
+      <selection activeCell="I43" sqref="I43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1039,7 +1029,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:35" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>35</v>
       </c>
@@ -1143,7 +1133,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:35" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>36</v>
       </c>
@@ -1247,7 +1237,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:35" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>37</v>
       </c>
@@ -1351,7 +1341,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:35" hidden="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>38</v>
       </c>
@@ -1455,7 +1445,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:35" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>39</v>
       </c>
@@ -1559,7 +1549,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:35" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>40</v>
       </c>
@@ -1775,7 +1765,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:35" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>41</v>
       </c>
@@ -1879,7 +1869,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:35" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>42</v>
       </c>
@@ -1983,7 +1973,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:35" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>43</v>
       </c>
@@ -2087,7 +2077,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:35" hidden="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>44</v>
       </c>
@@ -2191,7 +2181,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:35" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>45</v>
       </c>
@@ -2511,7 +2501,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:35" hidden="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>47</v>
       </c>
@@ -2719,7 +2709,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:35" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>49</v>
       </c>
@@ -2823,7 +2813,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:35" hidden="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>50</v>
       </c>
@@ -3143,7 +3133,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:35" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>52</v>
       </c>
@@ -3351,7 +3341,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:35" hidden="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>54</v>
       </c>
@@ -3455,7 +3445,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:35" hidden="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>55</v>
       </c>
@@ -3559,7 +3549,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:35" hidden="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>56</v>
       </c>
@@ -3879,7 +3869,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="38" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:35" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>58</v>
       </c>
@@ -3983,7 +3973,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:35" hidden="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>59</v>
       </c>
@@ -4087,7 +4077,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:35" hidden="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>60</v>
       </c>
@@ -4295,7 +4285,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:35" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>62</v>
       </c>
@@ -4615,7 +4605,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="47" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:35" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>64</v>
       </c>
@@ -4719,7 +4709,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:35" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>65</v>
       </c>
@@ -4823,7 +4813,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:35" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>66</v>
       </c>
@@ -5031,7 +5021,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:35" hidden="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>68</v>
       </c>
@@ -5135,7 +5125,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:35" hidden="1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>69</v>
       </c>

</xml_diff>